<commit_message>
Updated the example method, added the rest of the classes and updated the Individual Assessment file
</commit_message>
<xml_diff>
--- a/Individual Assessment.xlsx
+++ b/Individual Assessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karld\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karld\IdeaProjects\group-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E88D80-7F1A-469E-84D6-4F8857D44F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E500090-83C0-40F3-9993-B34FD3A10162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="3135" windowWidth="28800" windowHeight="15345" xr2:uid="{E82A4A5C-E753-4B05-8D34-C0B8E80B2BF5}"/>
+    <workbookView xWindow="1845" yWindow="4500" windowWidth="28785" windowHeight="15345" xr2:uid="{E82A4A5C-E753-4B05-8D34-C0B8E80B2BF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Matriculation Number</t>
   </si>
@@ -61,10 +61,13 @@
     <t>40443267 (Euan Campbell)</t>
   </si>
   <si>
-    <t>40443517 (Karl, Denison)</t>
-  </si>
-  <si>
     <t>40485296 (Usmaan Chohan)</t>
+  </si>
+  <si>
+    <t>40443517 (Karl Denison)</t>
+  </si>
+  <si>
+    <t>40491512 (Joe Black)</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE946AE-FC76-43D5-8C91-A4B5646A4464}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +468,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="4">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -474,10 +477,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -486,10 +489,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -498,26 +501,38 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="4">
         <v>100</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <v>100</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>100</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E6" s="4">
         <v>100</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F6" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>